<commit_message>
formatação cep e telefone
</commit_message>
<xml_diff>
--- a/clientes.xlsx
+++ b/clientes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -44,6 +44,12 @@
     <t>PE</t>
   </si>
   <si>
+    <t>54768-122</t>
+  </si>
+  <si>
+    <t>(12) 3456-678901</t>
+  </si>
+  <si>
     <t>Lucas</t>
   </si>
   <si>
@@ -53,6 +59,9 @@
     <t>RJ</t>
   </si>
   <si>
+    <t>(99) 3456-678901</t>
+  </si>
+  <si>
     <t>Bola</t>
   </si>
   <si>
@@ -60,6 +69,9 @@
   </si>
   <si>
     <t>BH</t>
+  </si>
+  <si>
+    <t>(99) 3456-678989</t>
   </si>
   <si>
     <t>Cabeça</t>
@@ -443,11 +455,11 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2">
-        <v>54768122</v>
-      </c>
-      <c r="F2">
-        <v>12345678901</v>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -455,19 +467,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3">
-        <v>54768122</v>
-      </c>
-      <c r="F3">
-        <v>99345678901</v>
+      <c r="F3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -475,19 +487,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4">
-        <v>54768122</v>
-      </c>
-      <c r="F4">
-        <v>99345678901</v>
+      <c r="F4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -495,19 +507,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5">
-        <v>54768122</v>
-      </c>
-      <c r="F5">
-        <v>99345678989</v>
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -515,19 +527,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6">
-        <v>54768122</v>
-      </c>
-      <c r="F6">
-        <v>99345678989</v>
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>